<commit_message>
update Edit RDP from file.rdp method
</commit_message>
<xml_diff>
--- a/Test_Suite/temp/settings_background.xlsx
+++ b/Test_Suite/temp/settings_background.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\Test_Suite\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1D951C-047B-4F16-B1EE-E850884745D4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83D920D-0E30-43F7-A228-3D98E289825C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>